<commit_message>
add account information when create a new role add init property module
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/EffectData.xlsx
+++ b/_Out/NFDataCfg/Excel/EffectData.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18528"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21495" windowHeight="10343"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21495" windowHeight="10343" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -432,7 +432,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -655,7 +655,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2">
-    <tableStyle name="MySqlDefault" count="1">
+    <tableStyle name="MySqlDefault" count="1" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
   </tableStyles>
@@ -998,14 +998,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="10" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="10" topLeftCell="Y11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G30" sqref="G30"/>
+      <selection pane="bottomRight" activeCell="AB11" sqref="AB11:AB70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1020,7 +1020,8 @@
     <col min="15" max="29" width="16.53125" customWidth="1"/>
     <col min="30" max="30" width="10.33203125" customWidth="1"/>
     <col min="31" max="31" width="13" customWidth="1"/>
-    <col min="32" max="33" width="12.1328125" customWidth="1"/>
+    <col min="32" max="32" width="12.1328125" customWidth="1"/>
+    <col min="33" max="33" width="15.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" s="1" customFormat="1">
@@ -2116,19 +2117,19 @@
         <v>50</v>
       </c>
       <c r="AB11">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC11">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD11">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE11">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF11">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG11">
         <v>0</v>
@@ -2217,19 +2218,19 @@
         <v>50</v>
       </c>
       <c r="AB12">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC12">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD12">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE12">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF12">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG12">
         <v>0</v>
@@ -2318,19 +2319,19 @@
         <v>50</v>
       </c>
       <c r="AB13">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC13">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD13">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE13">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF13">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG13">
         <v>0</v>
@@ -2419,19 +2420,19 @@
         <v>50</v>
       </c>
       <c r="AB14">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC14">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD14">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE14">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF14">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG14">
         <v>0</v>
@@ -2520,19 +2521,19 @@
         <v>50</v>
       </c>
       <c r="AB15">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC15">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD15">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE15">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF15">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG15">
         <v>0</v>
@@ -2621,19 +2622,19 @@
         <v>50</v>
       </c>
       <c r="AB16">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC16">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD16">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE16">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF16">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG16">
         <v>0</v>
@@ -2722,19 +2723,19 @@
         <v>50</v>
       </c>
       <c r="AB17">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC17">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD17">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE17">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF17">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG17">
         <v>0</v>
@@ -2823,19 +2824,19 @@
         <v>50</v>
       </c>
       <c r="AB18">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC18">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD18">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE18">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF18">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG18">
         <v>0</v>
@@ -2924,19 +2925,19 @@
         <v>50</v>
       </c>
       <c r="AB19">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC19">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD19">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE19">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF19">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG19">
         <v>0</v>
@@ -3025,19 +3026,19 @@
         <v>50</v>
       </c>
       <c r="AB20">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC20">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD20">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE20">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF20">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG20">
         <v>0</v>
@@ -3126,19 +3127,19 @@
         <v>50</v>
       </c>
       <c r="AB21">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC21">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD21">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE21">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF21">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG21">
         <v>0</v>
@@ -3227,19 +3228,19 @@
         <v>50</v>
       </c>
       <c r="AB22">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC22">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD22">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE22">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF22">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG22">
         <v>0</v>
@@ -3328,19 +3329,19 @@
         <v>50</v>
       </c>
       <c r="AB23">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC23">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD23">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE23">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF23">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG23">
         <v>0</v>
@@ -3429,19 +3430,19 @@
         <v>50</v>
       </c>
       <c r="AB24">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC24">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD24">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE24">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF24">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG24">
         <v>0</v>
@@ -3530,19 +3531,19 @@
         <v>50</v>
       </c>
       <c r="AB25">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC25">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD25">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE25">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF25">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG25">
         <v>0</v>
@@ -3631,19 +3632,19 @@
         <v>50</v>
       </c>
       <c r="AB26">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC26">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD26">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE26">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF26">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG26">
         <v>0</v>
@@ -3732,19 +3733,19 @@
         <v>50</v>
       </c>
       <c r="AB27">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC27">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD27">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE27">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF27">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG27">
         <v>0</v>
@@ -3833,19 +3834,19 @@
         <v>50</v>
       </c>
       <c r="AB28">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC28">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD28">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE28">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF28">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG28">
         <v>0</v>
@@ -3934,19 +3935,19 @@
         <v>50</v>
       </c>
       <c r="AB29">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC29">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD29">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE29">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF29">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG29">
         <v>0</v>
@@ -4035,19 +4036,19 @@
         <v>50</v>
       </c>
       <c r="AB30">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC30">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD30">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE30">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF30">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG30">
         <v>0</v>
@@ -4136,19 +4137,19 @@
         <v>50</v>
       </c>
       <c r="AB31">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC31">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD31">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE31">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF31">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG31">
         <v>0</v>
@@ -4237,19 +4238,19 @@
         <v>50</v>
       </c>
       <c r="AB32">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC32">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD32">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE32">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF32">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG32">
         <v>0</v>
@@ -4338,19 +4339,19 @@
         <v>50</v>
       </c>
       <c r="AB33">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC33">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD33">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE33">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF33">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG33">
         <v>0</v>
@@ -4439,19 +4440,19 @@
         <v>50</v>
       </c>
       <c r="AB34">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC34">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD34">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE34">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF34">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG34">
         <v>0</v>
@@ -4540,19 +4541,19 @@
         <v>50</v>
       </c>
       <c r="AB35">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC35">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD35">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE35">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF35">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG35">
         <v>0</v>
@@ -4641,19 +4642,19 @@
         <v>50</v>
       </c>
       <c r="AB36">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC36">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD36">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE36">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF36">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG36">
         <v>0</v>
@@ -4742,19 +4743,19 @@
         <v>50</v>
       </c>
       <c r="AB37">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC37">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD37">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE37">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF37">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG37">
         <v>0</v>
@@ -4843,19 +4844,19 @@
         <v>50</v>
       </c>
       <c r="AB38">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC38">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD38">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE38">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF38">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG38">
         <v>0</v>
@@ -4944,19 +4945,19 @@
         <v>50</v>
       </c>
       <c r="AB39">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC39">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD39">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE39">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF39">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG39">
         <v>0</v>
@@ -5045,19 +5046,19 @@
         <v>50</v>
       </c>
       <c r="AB40">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC40">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD40">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE40">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF40">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG40">
         <v>0</v>
@@ -5146,19 +5147,19 @@
         <v>50</v>
       </c>
       <c r="AB41">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC41">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD41">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE41">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF41">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG41">
         <v>0</v>
@@ -5247,19 +5248,19 @@
         <v>50</v>
       </c>
       <c r="AB42">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC42">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD42">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE42">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF42">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG42">
         <v>0</v>
@@ -5348,19 +5349,19 @@
         <v>50</v>
       </c>
       <c r="AB43">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC43">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD43">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE43">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF43">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG43">
         <v>0</v>
@@ -5449,19 +5450,19 @@
         <v>50</v>
       </c>
       <c r="AB44">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC44">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD44">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE44">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF44">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG44">
         <v>0</v>
@@ -5550,19 +5551,19 @@
         <v>50</v>
       </c>
       <c r="AB45">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC45">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD45">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE45">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF45">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG45">
         <v>0</v>
@@ -5651,19 +5652,19 @@
         <v>50</v>
       </c>
       <c r="AB46">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC46">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD46">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE46">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF46">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG46">
         <v>0</v>
@@ -5752,19 +5753,19 @@
         <v>50</v>
       </c>
       <c r="AB47">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC47">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD47">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE47">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF47">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG47">
         <v>0</v>
@@ -5853,19 +5854,19 @@
         <v>50</v>
       </c>
       <c r="AB48">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC48">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD48">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE48">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF48">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG48">
         <v>0</v>
@@ -5954,19 +5955,19 @@
         <v>50</v>
       </c>
       <c r="AB49">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC49">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD49">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE49">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF49">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG49">
         <v>0</v>
@@ -6055,19 +6056,19 @@
         <v>50</v>
       </c>
       <c r="AB50">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC50">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD50">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE50">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF50">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG50">
         <v>0</v>
@@ -6156,19 +6157,19 @@
         <v>50</v>
       </c>
       <c r="AB51">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC51">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD51">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE51">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF51">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG51">
         <v>0</v>
@@ -6257,19 +6258,19 @@
         <v>50</v>
       </c>
       <c r="AB52">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC52">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD52">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE52">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF52">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG52">
         <v>0</v>
@@ -6358,19 +6359,19 @@
         <v>50</v>
       </c>
       <c r="AB53">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC53">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD53">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE53">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF53">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG53">
         <v>0</v>
@@ -6459,19 +6460,19 @@
         <v>50</v>
       </c>
       <c r="AB54">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC54">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD54">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE54">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF54">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG54">
         <v>0</v>
@@ -6560,19 +6561,19 @@
         <v>50</v>
       </c>
       <c r="AB55">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC55">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD55">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE55">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF55">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG55">
         <v>0</v>
@@ -6661,19 +6662,19 @@
         <v>50</v>
       </c>
       <c r="AB56">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC56">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD56">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE56">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF56">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG56">
         <v>0</v>
@@ -6762,19 +6763,19 @@
         <v>50</v>
       </c>
       <c r="AB57">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC57">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD57">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE57">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF57">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG57">
         <v>0</v>
@@ -6863,19 +6864,19 @@
         <v>50</v>
       </c>
       <c r="AB58">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC58">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD58">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE58">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF58">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG58">
         <v>0</v>
@@ -6964,19 +6965,19 @@
         <v>50</v>
       </c>
       <c r="AB59">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC59">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD59">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE59">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF59">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG59">
         <v>0</v>
@@ -7065,19 +7066,19 @@
         <v>50</v>
       </c>
       <c r="AB60">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC60">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD60">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE60">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF60">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG60">
         <v>0</v>
@@ -7166,19 +7167,19 @@
         <v>50</v>
       </c>
       <c r="AB61">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC61">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD61">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE61">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF61">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG61">
         <v>0</v>
@@ -7267,19 +7268,19 @@
         <v>50</v>
       </c>
       <c r="AB62">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC62">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD62">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE62">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF62">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG62">
         <v>0</v>
@@ -7368,19 +7369,19 @@
         <v>50</v>
       </c>
       <c r="AB63">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC63">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD63">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE63">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF63">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG63">
         <v>0</v>
@@ -7469,19 +7470,19 @@
         <v>50</v>
       </c>
       <c r="AB64">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC64">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD64">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE64">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF64">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG64">
         <v>0</v>
@@ -7570,19 +7571,19 @@
         <v>50</v>
       </c>
       <c r="AB65">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC65">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD65">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE65">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF65">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG65">
         <v>0</v>
@@ -7671,19 +7672,19 @@
         <v>50</v>
       </c>
       <c r="AB66">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC66">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD66">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE66">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF66">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG66">
         <v>0</v>
@@ -7772,19 +7773,19 @@
         <v>50</v>
       </c>
       <c r="AB67">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC67">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD67">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE67">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF67">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG67">
         <v>0</v>
@@ -7873,19 +7874,19 @@
         <v>50</v>
       </c>
       <c r="AB68">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC68">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD68">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE68">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF68">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG68">
         <v>0</v>
@@ -7974,19 +7975,19 @@
         <v>50</v>
       </c>
       <c r="AB69">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC69">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD69">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE69">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF69">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG69">
         <v>0</v>
@@ -8075,19 +8076,19 @@
         <v>50</v>
       </c>
       <c r="AB70">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AC70">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AD70">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AE70">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AF70">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AG70">
         <v>0</v>
@@ -8095,8 +8096,8 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A9"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:AG9">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A9" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:AG9" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added size for the scene Fixed a bug for Datalist when serializing the data (ToString) Added a protocol for serializing the player position
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/EffectData.xlsx
+++ b/_Out/NFDataCfg/Excel/EffectData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21495" windowHeight="9930"/>
+    <workbookView windowWidth="21495" windowHeight="10335"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -550,8 +550,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="22">
@@ -570,14 +570,74 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -600,22 +660,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -628,32 +680,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -667,24 +704,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -695,28 +717,6 @@
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -741,7 +741,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -759,12 +837,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -777,19 +849,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -801,19 +897,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -826,102 +922,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1054,8 +1054,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1075,6 +1075,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1086,6 +1095,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1116,30 +1140,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1153,148 +1153,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1747,7 +1747,7 @@
   <dimension ref="A1:AG110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="10" topLeftCell="K90" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="10" topLeftCell="I99" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -2827,7 +2827,7 @@
         <v>0</v>
       </c>
       <c r="P11">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q11">
         <v>0</v>
@@ -2928,7 +2928,7 @@
         <v>50</v>
       </c>
       <c r="P12">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q12">
         <v>0</v>
@@ -3029,7 +3029,7 @@
         <v>100</v>
       </c>
       <c r="P13">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q13">
         <v>0</v>
@@ -3130,7 +3130,7 @@
         <v>150</v>
       </c>
       <c r="P14">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q14">
         <v>0</v>
@@ -3231,7 +3231,7 @@
         <v>200</v>
       </c>
       <c r="P15">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q15">
         <v>0</v>
@@ -3332,7 +3332,7 @@
         <v>250</v>
       </c>
       <c r="P16">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q16">
         <v>0</v>
@@ -3433,7 +3433,7 @@
         <v>300</v>
       </c>
       <c r="P17">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q17">
         <v>0</v>
@@ -3534,7 +3534,7 @@
         <v>350</v>
       </c>
       <c r="P18">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q18">
         <v>0</v>
@@ -3635,7 +3635,7 @@
         <v>400</v>
       </c>
       <c r="P19">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q19">
         <v>0</v>
@@ -3736,7 +3736,7 @@
         <v>450</v>
       </c>
       <c r="P20">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q20">
         <v>0</v>
@@ -3837,7 +3837,7 @@
         <v>500</v>
       </c>
       <c r="P21">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q21">
         <v>0</v>
@@ -3938,7 +3938,7 @@
         <v>550</v>
       </c>
       <c r="P22">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q22">
         <v>0</v>
@@ -4039,7 +4039,7 @@
         <v>600</v>
       </c>
       <c r="P23">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q23">
         <v>0</v>
@@ -4140,7 +4140,7 @@
         <v>650</v>
       </c>
       <c r="P24">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q24">
         <v>0</v>
@@ -4241,7 +4241,7 @@
         <v>700</v>
       </c>
       <c r="P25">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q25">
         <v>0</v>
@@ -4342,7 +4342,7 @@
         <v>750</v>
       </c>
       <c r="P26">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q26">
         <v>0</v>
@@ -4443,7 +4443,7 @@
         <v>800</v>
       </c>
       <c r="P27">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q27">
         <v>0</v>
@@ -4544,7 +4544,7 @@
         <v>850</v>
       </c>
       <c r="P28">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q28">
         <v>0</v>
@@ -4645,7 +4645,7 @@
         <v>900</v>
       </c>
       <c r="P29">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q29">
         <v>0</v>
@@ -4746,7 +4746,7 @@
         <v>950</v>
       </c>
       <c r="P30">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q30">
         <v>0</v>
@@ -4847,7 +4847,7 @@
         <v>1000</v>
       </c>
       <c r="P31">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q31">
         <v>0</v>
@@ -4948,7 +4948,7 @@
         <v>1050</v>
       </c>
       <c r="P32">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q32">
         <v>0</v>
@@ -5049,7 +5049,7 @@
         <v>1100</v>
       </c>
       <c r="P33">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q33">
         <v>0</v>
@@ -5150,7 +5150,7 @@
         <v>1150</v>
       </c>
       <c r="P34">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q34">
         <v>0</v>
@@ -5251,7 +5251,7 @@
         <v>1200</v>
       </c>
       <c r="P35">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q35">
         <v>0</v>
@@ -5352,7 +5352,7 @@
         <v>1250</v>
       </c>
       <c r="P36">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q36">
         <v>0</v>
@@ -5453,7 +5453,7 @@
         <v>1300</v>
       </c>
       <c r="P37">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q37">
         <v>0</v>
@@ -5554,7 +5554,7 @@
         <v>1350</v>
       </c>
       <c r="P38">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q38">
         <v>0</v>
@@ -5655,7 +5655,7 @@
         <v>1400</v>
       </c>
       <c r="P39">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q39">
         <v>0</v>
@@ -5756,7 +5756,7 @@
         <v>1450</v>
       </c>
       <c r="P40">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q40">
         <v>0</v>
@@ -5857,7 +5857,7 @@
         <v>1500</v>
       </c>
       <c r="P41">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q41">
         <v>0</v>
@@ -5958,7 +5958,7 @@
         <v>1550</v>
       </c>
       <c r="P42">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q42">
         <v>0</v>
@@ -6059,7 +6059,7 @@
         <v>1600</v>
       </c>
       <c r="P43">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q43">
         <v>0</v>
@@ -6160,7 +6160,7 @@
         <v>1650</v>
       </c>
       <c r="P44">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q44">
         <v>0</v>
@@ -6261,7 +6261,7 @@
         <v>1700</v>
       </c>
       <c r="P45">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q45">
         <v>0</v>
@@ -6362,7 +6362,7 @@
         <v>1750</v>
       </c>
       <c r="P46">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q46">
         <v>0</v>
@@ -6463,7 +6463,7 @@
         <v>1800</v>
       </c>
       <c r="P47">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q47">
         <v>0</v>
@@ -6564,7 +6564,7 @@
         <v>1850</v>
       </c>
       <c r="P48">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q48">
         <v>0</v>
@@ -6665,7 +6665,7 @@
         <v>1900</v>
       </c>
       <c r="P49">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q49">
         <v>0</v>
@@ -6766,7 +6766,7 @@
         <v>1950</v>
       </c>
       <c r="P50">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q50">
         <v>0</v>
@@ -6867,7 +6867,7 @@
         <v>2000</v>
       </c>
       <c r="P51">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q51">
         <v>0</v>
@@ -6968,7 +6968,7 @@
         <v>2050</v>
       </c>
       <c r="P52">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q52">
         <v>0</v>
@@ -7069,7 +7069,7 @@
         <v>2100</v>
       </c>
       <c r="P53">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q53">
         <v>0</v>
@@ -7170,7 +7170,7 @@
         <v>2150</v>
       </c>
       <c r="P54">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q54">
         <v>0</v>
@@ -7271,7 +7271,7 @@
         <v>2200</v>
       </c>
       <c r="P55">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q55">
         <v>0</v>
@@ -7372,7 +7372,7 @@
         <v>2250</v>
       </c>
       <c r="P56">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q56">
         <v>0</v>
@@ -7473,7 +7473,7 @@
         <v>2300</v>
       </c>
       <c r="P57">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q57">
         <v>0</v>
@@ -7574,7 +7574,7 @@
         <v>2350</v>
       </c>
       <c r="P58">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q58">
         <v>0</v>
@@ -7675,7 +7675,7 @@
         <v>2400</v>
       </c>
       <c r="P59">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q59">
         <v>0</v>
@@ -7776,7 +7776,7 @@
         <v>2450</v>
       </c>
       <c r="P60">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q60">
         <v>0</v>
@@ -7877,7 +7877,7 @@
         <v>2500</v>
       </c>
       <c r="P61">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q61">
         <v>0</v>
@@ -7978,7 +7978,7 @@
         <v>2550</v>
       </c>
       <c r="P62">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q62">
         <v>0</v>
@@ -8079,7 +8079,7 @@
         <v>2600</v>
       </c>
       <c r="P63">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q63">
         <v>0</v>
@@ -8180,7 +8180,7 @@
         <v>2650</v>
       </c>
       <c r="P64">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q64">
         <v>0</v>
@@ -8281,7 +8281,7 @@
         <v>2700</v>
       </c>
       <c r="P65">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q65">
         <v>0</v>
@@ -8382,7 +8382,7 @@
         <v>2750</v>
       </c>
       <c r="P66">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q66">
         <v>0</v>
@@ -8483,7 +8483,7 @@
         <v>2800</v>
       </c>
       <c r="P67">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q67">
         <v>0</v>
@@ -8584,7 +8584,7 @@
         <v>2850</v>
       </c>
       <c r="P68">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q68">
         <v>0</v>
@@ -8685,7 +8685,7 @@
         <v>2900</v>
       </c>
       <c r="P69">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q69">
         <v>0</v>
@@ -8786,7 +8786,7 @@
         <v>2950</v>
       </c>
       <c r="P70">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q70">
         <v>0</v>
@@ -8887,7 +8887,7 @@
         <v>3000</v>
       </c>
       <c r="P71">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q71">
         <v>0</v>
@@ -8988,7 +8988,7 @@
         <v>3050</v>
       </c>
       <c r="P72">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q72">
         <v>0</v>
@@ -9089,7 +9089,7 @@
         <v>3100</v>
       </c>
       <c r="P73">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q73">
         <v>0</v>
@@ -9190,7 +9190,7 @@
         <v>3150</v>
       </c>
       <c r="P74">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q74">
         <v>0</v>
@@ -9291,7 +9291,7 @@
         <v>3200</v>
       </c>
       <c r="P75">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q75">
         <v>0</v>
@@ -9392,7 +9392,7 @@
         <v>3250</v>
       </c>
       <c r="P76">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q76">
         <v>0</v>
@@ -9493,7 +9493,7 @@
         <v>3300</v>
       </c>
       <c r="P77">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q77">
         <v>0</v>
@@ -9594,7 +9594,7 @@
         <v>3350</v>
       </c>
       <c r="P78">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q78">
         <v>0</v>
@@ -9695,7 +9695,7 @@
         <v>3400</v>
       </c>
       <c r="P79">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q79">
         <v>0</v>
@@ -9796,7 +9796,7 @@
         <v>3450</v>
       </c>
       <c r="P80">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q80">
         <v>0</v>
@@ -9897,7 +9897,7 @@
         <v>3500</v>
       </c>
       <c r="P81">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q81">
         <v>0</v>
@@ -9998,7 +9998,7 @@
         <v>3550</v>
       </c>
       <c r="P82">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q82">
         <v>0</v>
@@ -10099,7 +10099,7 @@
         <v>3600</v>
       </c>
       <c r="P83">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q83">
         <v>0</v>
@@ -10200,7 +10200,7 @@
         <v>3650</v>
       </c>
       <c r="P84">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q84">
         <v>0</v>
@@ -10301,7 +10301,7 @@
         <v>3700</v>
       </c>
       <c r="P85">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q85">
         <v>0</v>
@@ -10402,7 +10402,7 @@
         <v>3750</v>
       </c>
       <c r="P86">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q86">
         <v>0</v>
@@ -10503,7 +10503,7 @@
         <v>3800</v>
       </c>
       <c r="P87">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q87">
         <v>0</v>
@@ -10604,7 +10604,7 @@
         <v>3850</v>
       </c>
       <c r="P88">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q88">
         <v>0</v>
@@ -10705,7 +10705,7 @@
         <v>3900</v>
       </c>
       <c r="P89">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q89">
         <v>0</v>
@@ -10806,7 +10806,7 @@
         <v>3950</v>
       </c>
       <c r="P90">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q90">
         <v>0</v>
@@ -10907,7 +10907,7 @@
         <v>4000</v>
       </c>
       <c r="P91">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q91">
         <v>0</v>
@@ -11008,7 +11008,7 @@
         <v>4050</v>
       </c>
       <c r="P92">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q92">
         <v>0</v>
@@ -11109,7 +11109,7 @@
         <v>4100</v>
       </c>
       <c r="P93">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q93">
         <v>0</v>
@@ -11210,7 +11210,7 @@
         <v>4150</v>
       </c>
       <c r="P94">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q94">
         <v>0</v>
@@ -11311,7 +11311,7 @@
         <v>4200</v>
       </c>
       <c r="P95">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q95">
         <v>0</v>
@@ -11412,7 +11412,7 @@
         <v>4250</v>
       </c>
       <c r="P96">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q96">
         <v>0</v>
@@ -11513,7 +11513,7 @@
         <v>4300</v>
       </c>
       <c r="P97">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q97">
         <v>0</v>
@@ -11614,7 +11614,7 @@
         <v>4350</v>
       </c>
       <c r="P98">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q98">
         <v>0</v>
@@ -11715,7 +11715,7 @@
         <v>4400</v>
       </c>
       <c r="P99">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q99">
         <v>0</v>
@@ -11816,7 +11816,7 @@
         <v>4450</v>
       </c>
       <c r="P100">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q100">
         <v>0</v>
@@ -11917,7 +11917,7 @@
         <v>4500</v>
       </c>
       <c r="P101">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q101">
         <v>0</v>
@@ -12018,7 +12018,7 @@
         <v>4550</v>
       </c>
       <c r="P102">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q102">
         <v>0</v>
@@ -12119,7 +12119,7 @@
         <v>4600</v>
       </c>
       <c r="P103">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q103">
         <v>0</v>
@@ -12220,7 +12220,7 @@
         <v>4650</v>
       </c>
       <c r="P104">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q104">
         <v>0</v>
@@ -12321,7 +12321,7 @@
         <v>4700</v>
       </c>
       <c r="P105">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q105">
         <v>0</v>
@@ -12422,7 +12422,7 @@
         <v>4750</v>
       </c>
       <c r="P106">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q106">
         <v>0</v>
@@ -12523,7 +12523,7 @@
         <v>4800</v>
       </c>
       <c r="P107">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q107">
         <v>0</v>
@@ -12624,7 +12624,7 @@
         <v>4850</v>
       </c>
       <c r="P108">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q108">
         <v>0</v>
@@ -12725,7 +12725,7 @@
         <v>4900</v>
       </c>
       <c r="P109">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q109">
         <v>0</v>
@@ -12826,7 +12826,7 @@
         <v>4950</v>
       </c>
       <c r="P110">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="Q110">
         <v>0</v>

</xml_diff>